<commit_message>
Re-tuned gains to correct formula
-.1 -.001 -3; added throttle input as an input variable in main()
</commit_message>
<xml_diff>
--- a/Gains_trials.xlsx
+++ b/Gains_trials.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>kp</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t xml:space="preserve">passed 3 laps ! </t>
+  </si>
+  <si>
+    <t>up throttle to 0.3</t>
+  </si>
+  <si>
+    <t>up throttle to 0.35</t>
+  </si>
+  <si>
+    <t>Found a mistake in my code which, reset throttle to 0.25</t>
+  </si>
+  <si>
+    <t>Crazy Osclilations</t>
   </si>
 </sst>
 </file>
@@ -432,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6442C2BA-6ACC-4173-97B4-5E5DDDEAC34F}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,6 +827,96 @@
         <v>18</v>
       </c>
     </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>-0.1</v>
+      </c>
+      <c r="B30">
+        <v>1E-3</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>-0.1</v>
+      </c>
+      <c r="B32">
+        <v>1E-3</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>-0.1</v>
+      </c>
+      <c r="B34">
+        <v>1E-3</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>-0.1</v>
+      </c>
+      <c r="B36">
+        <v>1E-3</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>-0.1</v>
+      </c>
+      <c r="B37">
+        <v>-1E-3</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Increased Throttle to 0.7
</commit_message>
<xml_diff>
--- a/Gains_trials.xlsx
+++ b/Gains_trials.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>kp</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>Crazy Osclilations</t>
+  </si>
+  <si>
+    <t>Oscilates a lot at the start but once it picks up speed the behavior is very smooth. Passed !</t>
+  </si>
+  <si>
+    <t>passed 3 laps !</t>
+  </si>
+  <si>
+    <t>up throttle to 0.5</t>
+  </si>
+  <si>
+    <t>passed 3 laps! Top speed 57 mph</t>
   </si>
 </sst>
 </file>
@@ -444,15 +456,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6442C2BA-6ACC-4173-97B4-5E5DDDEAC34F}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="41.6640625" customWidth="1"/>
+    <col min="4" max="4" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -743,7 +755,7 @@
         <v>-0.1</v>
       </c>
       <c r="B22">
-        <v>5.0000000000000001E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -757,7 +769,7 @@
         <v>-0.1</v>
       </c>
       <c r="B23">
-        <v>5.0000000000000001E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -771,7 +783,7 @@
         <v>-0.1</v>
       </c>
       <c r="B24">
-        <v>5.0000000000000001E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -785,7 +797,7 @@
         <v>-0.1</v>
       </c>
       <c r="B25">
-        <v>5.0000000000000001E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -799,7 +811,7 @@
         <v>-0.1</v>
       </c>
       <c r="B26">
-        <v>1E-3</v>
+        <v>-1E-3</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -818,7 +830,7 @@
         <v>-0.1</v>
       </c>
       <c r="B28">
-        <v>1E-3</v>
+        <v>-1E-3</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -837,7 +849,7 @@
         <v>-0.1</v>
       </c>
       <c r="B30">
-        <v>1E-3</v>
+        <v>-1E-3</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -856,7 +868,7 @@
         <v>-0.1</v>
       </c>
       <c r="B32">
-        <v>1E-3</v>
+        <v>-1E-3</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -875,7 +887,7 @@
         <v>-0.1</v>
       </c>
       <c r="B34">
-        <v>1E-3</v>
+        <v>-1E-3</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -894,7 +906,7 @@
         <v>-0.1</v>
       </c>
       <c r="B36">
-        <v>1E-3</v>
+        <v>-1E-3</v>
       </c>
       <c r="C36">
         <v>3</v>
@@ -915,6 +927,77 @@
       </c>
       <c r="D37" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>-0.1</v>
+      </c>
+      <c r="B38">
+        <v>-1E-4</v>
+      </c>
+      <c r="C38">
+        <v>-3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>-0.1</v>
+      </c>
+      <c r="B40">
+        <v>-1E-4</v>
+      </c>
+      <c r="C40">
+        <v>-3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>-0.1</v>
+      </c>
+      <c r="B42">
+        <v>-1E-4</v>
+      </c>
+      <c r="C42">
+        <v>-3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>-0.1</v>
+      </c>
+      <c r="B44">
+        <v>-1E-4</v>
+      </c>
+      <c r="C44">
+        <v>-3</v>
+      </c>
+      <c r="D44" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Harcoded the gains & the set Speed
</commit_message>
<xml_diff>
--- a/Gains_trials.xlsx
+++ b/Gains_trials.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13584" windowHeight="5640" xr2:uid="{659158FA-3E24-4C41-8B03-FFF63F4FA36E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="5640" activeTab="1" xr2:uid="{659158FA-3E24-4C41-8B03-FFF63F4FA36E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PID cte &amp; Vel" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>kp</t>
   </si>
@@ -105,6 +106,54 @@
   </si>
   <si>
     <t>passed 3 laps! Top speed 57 mph</t>
+  </si>
+  <si>
+    <t>up throttle to 0.7</t>
+  </si>
+  <si>
+    <t>passed 3 laps! Top speed 77 mph. oscilatory behavior coming out of turns</t>
+  </si>
+  <si>
+    <t>passed 3 laps! Top speed 75 mph. oscilatory behavior coming out of turns</t>
+  </si>
+  <si>
+    <t>Crash</t>
+  </si>
+  <si>
+    <t>passed 3 laps! Top speed 74 mph. oscilatory behavior coming out of turns</t>
+  </si>
+  <si>
+    <t>passed 3 laps! Top speed 78 mph. oscilatory behavior coming out of turns</t>
+  </si>
+  <si>
+    <t>passed 3 laps! Top speed 78 mph. oscilatory behavior coming out of turns, no oscilations at the start.</t>
+  </si>
+  <si>
+    <t>passed 3 laps! Top speed 78.6 mph. oscilatory behavior coming out of turns, no oscilations at the start.</t>
+  </si>
+  <si>
+    <t>Cte</t>
+  </si>
+  <si>
+    <t>vel</t>
+  </si>
+  <si>
+    <t>lol , K should be + positive, started driving in reserve for the course, not bad though</t>
+  </si>
+  <si>
+    <t>Passed !  Driving is a lot smother. Very sligth bias error -0.4 Time to up the spped to 25.0.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed </t>
+  </si>
+  <si>
+    <t>Passed !  Driving is a lot smother. Very sligth bias error -0.3</t>
+  </si>
+  <si>
+    <t>Passed !  Driving is a lot smother. Very sligth bias error -0.4</t>
+  </si>
+  <si>
+    <t>Passed !  Driving is a lot smother. Very sligth bias error -0.4, osclilatory behavior out of the bends.</t>
   </si>
 </sst>
 </file>
@@ -140,8 +189,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6442C2BA-6ACC-4173-97B4-5E5DDDEAC34F}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,7 +1055,380 @@
         <v>26</v>
       </c>
     </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>-0.1</v>
+      </c>
+      <c r="B46">
+        <v>-1E-4</v>
+      </c>
+      <c r="C46">
+        <v>-3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>-0.1</v>
+      </c>
+      <c r="B47">
+        <v>-1E-4</v>
+      </c>
+      <c r="C47">
+        <v>-3.5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>-0.1</v>
+      </c>
+      <c r="B48">
+        <v>-1E-4</v>
+      </c>
+      <c r="C48">
+        <v>-5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>-0.1</v>
+      </c>
+      <c r="B49">
+        <v>-1E-4</v>
+      </c>
+      <c r="C49">
+        <v>-2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>-0.1</v>
+      </c>
+      <c r="B50">
+        <v>-1E-4</v>
+      </c>
+      <c r="C50">
+        <v>-6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>-0.1</v>
+      </c>
+      <c r="B51">
+        <v>-1E-4</v>
+      </c>
+      <c r="C51">
+        <v>-3.2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>-0.1</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>-3.2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>-0.1</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>-2.8</v>
+      </c>
+      <c r="D53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>-0.11</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>-3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A22F92-EE1B-4BF4-ACF0-E113833E1B54}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="56.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>-0.11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>-3</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>-0.11</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>-3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>-0.11</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>-3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>-0.11</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>-3</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>-0.11</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>-3</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>50</v>
+      </c>
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>-0.11</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>-3</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>70</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>-0.11</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>-4</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>70</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
double check before submission
</commit_message>
<xml_diff>
--- a/Gains_trials.xlsx
+++ b/Gains_trials.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
   <si>
     <t>kp</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Passed !  Driving is a lot smother. Very sligth bias error -0.4, osclilatory behavior out of the bends.</t>
+  </si>
+  <si>
+    <t>Good response</t>
+  </si>
+  <si>
+    <t>Good response,  bias error below .03</t>
   </si>
 </sst>
 </file>
@@ -513,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6442C2BA-6ACC-4173-97B4-5E5DDDEAC34F}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
@@ -1193,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A22F92-EE1B-4BF4-ACF0-E113833E1B54}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1424,6 +1430,84 @@
         <v>42</v>
       </c>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>-0.11</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>-4</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1E-3</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>-0.11</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>-4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>-0.11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>-4</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>50</v>
+      </c>
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>

</xml_diff>